<commit_message>
Fix some bugs and add dashboard
</commit_message>
<xml_diff>
--- a/public/templates/tools-template.xlsx
+++ b/public/templates/tools-template.xlsx
@@ -16,16 +16,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
-    <t>Equipment</t>
-  </si>
-  <si>
-    <t>TechIdentNo.</t>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>Tech Ident Number</t>
   </si>
   <si>
     <t>Business Area</t>
   </si>
   <si>
-    <t>MaintPlant</t>
+    <t>Maintenance Plant</t>
   </si>
   <si>
     <t>Material</t>
@@ -34,16 +34,16 @@
     <t>Manufacturer</t>
   </si>
   <si>
-    <t>Title Description</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Size/dimens.</t>
-  </si>
-  <si>
-    <t>ManufSerialNo.</t>
+    <t>Additional Description</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Manufacture Serial Number</t>
   </si>
   <si>
     <t>Asset</t>
@@ -52,7 +52,7 @@
     <t>Location</t>
   </si>
   <si>
-    <t>License no.</t>
+    <t>License Number</t>
   </si>
   <si>
     <t>System status</t>
@@ -64,16 +64,16 @@
     <t>Sort field</t>
   </si>
   <si>
-    <t>EquipCategory</t>
+    <t>Equipment Category</t>
   </si>
   <si>
     <t>Currency</t>
   </si>
   <si>
-    <t>AcquistnValue</t>
-  </si>
-  <si>
-    <t>Start-up date</t>
+    <t>Acquisition Value</t>
+  </si>
+  <si>
+    <t>Start Up date</t>
   </si>
   <si>
     <t>Changed by</t>
@@ -85,10 +85,10 @@
     <t>Created by</t>
   </si>
   <si>
-    <t>ABC indic.</t>
-  </si>
-  <si>
-    <t>Acquistion date</t>
+    <t>ABC indic</t>
+  </si>
+  <si>
+    <t>Acquisition date</t>
   </si>
   <si>
     <t>10103686</t>
@@ -153,9 +153,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
@@ -176,15 +176,16 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -206,106 +207,105 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -338,181 +338,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -531,15 +531,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -564,21 +555,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -623,87 +599,111 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -712,58 +712,58 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1109,8 +1109,8 @@
   <sheetPr/>
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>

</xml_diff>